<commit_message>
akaunting 3.0 (the last dance)
</commit_message>
<xml_diff>
--- a/public/files/import/categories.xlsx
+++ b/public/files/import/categories.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cihan Ş\Desktop\software-import-sample\public\files\import\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9204"/>
   </bookViews>
   <sheets>
-    <sheet name="categories" sheetId="1" r:id="rId4"/>
+    <sheet name="categories" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1" forceFullCalc="1"/>
+  <calcPr calcId="162913" forceFullCalc="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>name</t>
   </si>
@@ -75,19 +79,17 @@
   </si>
   <si>
     <t>#3f317</t>
+  </si>
+  <si>
+    <t>TRUE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <b val="0"/>
-      <i val="0"/>
-      <strike val="0"/>
-      <u val="none"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -98,28 +100,37 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -409,25 +420,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.568848" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="9.283447" bestFit="true" customWidth="true" style="0"/>
-    <col min="3" max="3" width="9.283447" bestFit="true" customWidth="true" style="0"/>
-    <col min="4" max="4" width="9.283447" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,7 +447,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -451,11 +457,11 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -465,11 +471,11 @@
       <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -479,11 +485,11 @@
       <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -493,11 +499,11 @@
       <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -507,11 +513,11 @@
       <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -521,22 +527,17 @@
       <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="D7" t="b">
-        <v>1</v>
+      <c r="D7" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Enabled Error" error="You must choose true or false" sqref="D2:D1048576">
+      <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
categories import sample file type field development
</commit_message>
<xml_diff>
--- a/public/files/import/categories.xlsx
+++ b/public/files/import/categories.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cihan Ş\Desktop\software-import-sample\public\files\import\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9204"/>
+    <workbookView windowWidth="28800" windowHeight="12495"/>
   </bookViews>
   <sheets>
     <sheet name="categories" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" forceFullCalc="1"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -42,6 +37,9 @@
     <t>#3c3f72</t>
   </si>
   <si>
+    <t>TRUE</t>
+  </si>
+  <si>
     <t>Deposit</t>
   </si>
   <si>
@@ -79,31 +77,372 @@
   </si>
   <si>
     <t>#3f317</t>
-  </si>
-  <si>
-    <t>TRUE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -111,24 +450,310 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
+    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
+    <cellStyle name="Note" xfId="12" builtinId="10"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -415,25 +1040,25 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.552380952381" customWidth="1"/>
+    <col min="2" max="4" width="9.33333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -447,7 +1072,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -458,86 +1083,90 @@
         <v>6</v>
       </c>
       <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="D7" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <dataValidations count="1">
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576">
+      <formula1>"expense,income,item,other,ticket,asset,contracts"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Enabled Error" error="You must choose true or false" sqref="D2:D1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>